<commit_message>
Started review #1 and changes from Leonardo
</commit_message>
<xml_diff>
--- a/assets/gantt-diagram.xlsx
+++ b/assets/gantt-diagram.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C1A237A-7472-4F99-81B4-FDE78AE43B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04EFB55D-5D38-4B36-A890-3D1F73ACDA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="76">
   <si>
     <t>Create a Project Schedule in this worksheet.
 Enter title of this project in cell B1. 
@@ -293,6 +293,15 @@
   <si>
     <t>Requirements</t>
   </si>
+  <si>
+    <t>Final Report</t>
+  </si>
+  <si>
+    <t>Write Up</t>
+  </si>
+  <si>
+    <t>Task 11</t>
+  </si>
 </sst>
 </file>
 
@@ -539,7 +548,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="49">
+  <fills count="50">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -812,6 +821,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1088,7 +1103,7 @@
     <xf numFmtId="0" fontId="9" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1381,6 +1396,13 @@
     <xf numFmtId="168" fontId="9" fillId="7" borderId="0" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" xfId="19"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
     <xf numFmtId="169" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1390,17 +1412,22 @@
     <xf numFmtId="169" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" xfId="19"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="19" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="49" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="49" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="49" borderId="2" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="49" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="54">
     <cellStyle name="20% - Accent1" xfId="31" builtinId="30" customBuiltin="1"/>
@@ -1458,44 +1485,11 @@
     <cellStyle name="Warning Text" xfId="26" builtinId="11" customBuiltin="1"/>
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="13">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0066"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
       <border>
@@ -1636,15 +1630,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="15"/>
-      <tableStyleElement type="headerRow" dxfId="14"/>
-      <tableStyleElement type="totalRow" dxfId="13"/>
-      <tableStyleElement type="firstColumn" dxfId="12"/>
-      <tableStyleElement type="lastColumn" dxfId="11"/>
-      <tableStyleElement type="firstRowStripe" dxfId="10"/>
-      <tableStyleElement type="secondRowStripe" dxfId="9"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="8"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="7"/>
+      <tableStyleElement type="wholeTable" dxfId="12"/>
+      <tableStyleElement type="headerRow" dxfId="11"/>
+      <tableStyleElement type="totalRow" dxfId="10"/>
+      <tableStyleElement type="firstColumn" dxfId="9"/>
+      <tableStyleElement type="lastColumn" dxfId="8"/>
+      <tableStyleElement type="firstRowStripe" dxfId="7"/>
+      <tableStyleElement type="secondRowStripe" dxfId="6"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="5"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="4"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2004,13 +1998,13 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:HD50"/>
+  <dimension ref="A1:HD52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane xSplit="8" ySplit="7" topLeftCell="I8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="7" topLeftCell="BZ38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight" activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2096,15 +2090,15 @@
       <c r="BQ2" s="111"/>
       <c r="BR2" s="111"/>
       <c r="BS2" s="111"/>
-      <c r="GX2" s="107" t="s">
+      <c r="GX2" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="GY2" s="107"/>
-      <c r="GZ2" s="107"/>
-      <c r="HA2" s="107"/>
-      <c r="HB2" s="107"/>
-      <c r="HC2" s="107"/>
-      <c r="HD2" s="107"/>
+      <c r="GY2" s="104"/>
+      <c r="GZ2" s="104"/>
+      <c r="HA2" s="104"/>
+      <c r="HB2" s="104"/>
+      <c r="HC2" s="104"/>
+      <c r="HD2" s="104"/>
     </row>
     <row r="3" spans="1:212" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="34" t="s">
@@ -2113,10 +2107,10 @@
       <c r="B3" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="108" t="s">
+      <c r="C3" s="105" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="109"/>
+      <c r="D3" s="106"/>
       <c r="E3" s="110">
         <v>44851</v>
       </c>
@@ -2126,303 +2120,303 @@
       <c r="A4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="108" t="s">
+      <c r="C4" s="105" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="109"/>
+      <c r="D4" s="106"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="104">
+      <c r="I4" s="107">
         <f>I5</f>
         <v>44851</v>
       </c>
-      <c r="J4" s="105"/>
-      <c r="K4" s="105"/>
-      <c r="L4" s="105"/>
-      <c r="M4" s="105"/>
-      <c r="N4" s="105"/>
-      <c r="O4" s="106"/>
-      <c r="P4" s="104">
+      <c r="J4" s="108"/>
+      <c r="K4" s="108"/>
+      <c r="L4" s="108"/>
+      <c r="M4" s="108"/>
+      <c r="N4" s="108"/>
+      <c r="O4" s="109"/>
+      <c r="P4" s="107">
         <f>P5</f>
         <v>44858</v>
       </c>
-      <c r="Q4" s="105"/>
-      <c r="R4" s="105"/>
-      <c r="S4" s="105"/>
-      <c r="T4" s="105"/>
-      <c r="U4" s="105"/>
-      <c r="V4" s="106"/>
-      <c r="W4" s="104">
+      <c r="Q4" s="108"/>
+      <c r="R4" s="108"/>
+      <c r="S4" s="108"/>
+      <c r="T4" s="108"/>
+      <c r="U4" s="108"/>
+      <c r="V4" s="109"/>
+      <c r="W4" s="107">
         <f>W5</f>
         <v>44865</v>
       </c>
-      <c r="X4" s="105"/>
-      <c r="Y4" s="105"/>
-      <c r="Z4" s="105"/>
-      <c r="AA4" s="105"/>
-      <c r="AB4" s="105"/>
-      <c r="AC4" s="106"/>
-      <c r="AD4" s="104">
+      <c r="X4" s="108"/>
+      <c r="Y4" s="108"/>
+      <c r="Z4" s="108"/>
+      <c r="AA4" s="108"/>
+      <c r="AB4" s="108"/>
+      <c r="AC4" s="109"/>
+      <c r="AD4" s="107">
         <f>AD5</f>
         <v>44872</v>
       </c>
-      <c r="AE4" s="105"/>
-      <c r="AF4" s="105"/>
-      <c r="AG4" s="105"/>
-      <c r="AH4" s="105"/>
-      <c r="AI4" s="105"/>
-      <c r="AJ4" s="106"/>
-      <c r="AK4" s="104">
+      <c r="AE4" s="108"/>
+      <c r="AF4" s="108"/>
+      <c r="AG4" s="108"/>
+      <c r="AH4" s="108"/>
+      <c r="AI4" s="108"/>
+      <c r="AJ4" s="109"/>
+      <c r="AK4" s="107">
         <f>AK5</f>
         <v>44879</v>
       </c>
-      <c r="AL4" s="105"/>
-      <c r="AM4" s="105"/>
-      <c r="AN4" s="105"/>
-      <c r="AO4" s="105"/>
-      <c r="AP4" s="105"/>
-      <c r="AQ4" s="106"/>
-      <c r="AR4" s="104">
+      <c r="AL4" s="108"/>
+      <c r="AM4" s="108"/>
+      <c r="AN4" s="108"/>
+      <c r="AO4" s="108"/>
+      <c r="AP4" s="108"/>
+      <c r="AQ4" s="109"/>
+      <c r="AR4" s="107">
         <f>AR5</f>
         <v>44886</v>
       </c>
-      <c r="AS4" s="105"/>
-      <c r="AT4" s="105"/>
-      <c r="AU4" s="105"/>
-      <c r="AV4" s="105"/>
-      <c r="AW4" s="105"/>
-      <c r="AX4" s="106"/>
-      <c r="AY4" s="104">
+      <c r="AS4" s="108"/>
+      <c r="AT4" s="108"/>
+      <c r="AU4" s="108"/>
+      <c r="AV4" s="108"/>
+      <c r="AW4" s="108"/>
+      <c r="AX4" s="109"/>
+      <c r="AY4" s="107">
         <f>AY5</f>
         <v>44893</v>
       </c>
-      <c r="AZ4" s="105"/>
-      <c r="BA4" s="105"/>
-      <c r="BB4" s="105"/>
-      <c r="BC4" s="105"/>
-      <c r="BD4" s="105"/>
-      <c r="BE4" s="106"/>
-      <c r="BF4" s="104">
+      <c r="AZ4" s="108"/>
+      <c r="BA4" s="108"/>
+      <c r="BB4" s="108"/>
+      <c r="BC4" s="108"/>
+      <c r="BD4" s="108"/>
+      <c r="BE4" s="109"/>
+      <c r="BF4" s="107">
         <f>BF5</f>
         <v>44900</v>
       </c>
-      <c r="BG4" s="105"/>
-      <c r="BH4" s="105"/>
-      <c r="BI4" s="105"/>
-      <c r="BJ4" s="105"/>
-      <c r="BK4" s="105"/>
-      <c r="BL4" s="106"/>
-      <c r="BM4" s="104">
+      <c r="BG4" s="108"/>
+      <c r="BH4" s="108"/>
+      <c r="BI4" s="108"/>
+      <c r="BJ4" s="108"/>
+      <c r="BK4" s="108"/>
+      <c r="BL4" s="109"/>
+      <c r="BM4" s="107">
         <f>BM5</f>
         <v>44907</v>
       </c>
-      <c r="BN4" s="105"/>
-      <c r="BO4" s="105"/>
-      <c r="BP4" s="105"/>
-      <c r="BQ4" s="105"/>
-      <c r="BR4" s="105"/>
-      <c r="BS4" s="106"/>
-      <c r="BT4" s="104">
+      <c r="BN4" s="108"/>
+      <c r="BO4" s="108"/>
+      <c r="BP4" s="108"/>
+      <c r="BQ4" s="108"/>
+      <c r="BR4" s="108"/>
+      <c r="BS4" s="109"/>
+      <c r="BT4" s="107">
         <f>BT5</f>
         <v>44914</v>
       </c>
-      <c r="BU4" s="105"/>
-      <c r="BV4" s="105"/>
-      <c r="BW4" s="105"/>
-      <c r="BX4" s="105"/>
-      <c r="BY4" s="105"/>
-      <c r="BZ4" s="106"/>
-      <c r="CA4" s="104">
+      <c r="BU4" s="108"/>
+      <c r="BV4" s="108"/>
+      <c r="BW4" s="108"/>
+      <c r="BX4" s="108"/>
+      <c r="BY4" s="108"/>
+      <c r="BZ4" s="109"/>
+      <c r="CA4" s="107">
         <f>CA5</f>
         <v>44921</v>
       </c>
-      <c r="CB4" s="105"/>
-      <c r="CC4" s="105"/>
-      <c r="CD4" s="105"/>
-      <c r="CE4" s="105"/>
-      <c r="CF4" s="105"/>
-      <c r="CG4" s="106"/>
-      <c r="CH4" s="104">
+      <c r="CB4" s="108"/>
+      <c r="CC4" s="108"/>
+      <c r="CD4" s="108"/>
+      <c r="CE4" s="108"/>
+      <c r="CF4" s="108"/>
+      <c r="CG4" s="109"/>
+      <c r="CH4" s="107">
         <f>CH5</f>
         <v>44928</v>
       </c>
-      <c r="CI4" s="105"/>
-      <c r="CJ4" s="105"/>
-      <c r="CK4" s="105"/>
-      <c r="CL4" s="105"/>
-      <c r="CM4" s="105"/>
-      <c r="CN4" s="106"/>
-      <c r="CO4" s="104">
+      <c r="CI4" s="108"/>
+      <c r="CJ4" s="108"/>
+      <c r="CK4" s="108"/>
+      <c r="CL4" s="108"/>
+      <c r="CM4" s="108"/>
+      <c r="CN4" s="109"/>
+      <c r="CO4" s="107">
         <f>CO5</f>
         <v>44935</v>
       </c>
-      <c r="CP4" s="105"/>
-      <c r="CQ4" s="105"/>
-      <c r="CR4" s="105"/>
-      <c r="CS4" s="105"/>
-      <c r="CT4" s="105"/>
-      <c r="CU4" s="106"/>
-      <c r="CV4" s="104">
+      <c r="CP4" s="108"/>
+      <c r="CQ4" s="108"/>
+      <c r="CR4" s="108"/>
+      <c r="CS4" s="108"/>
+      <c r="CT4" s="108"/>
+      <c r="CU4" s="109"/>
+      <c r="CV4" s="107">
         <f>CV5</f>
         <v>44942</v>
       </c>
-      <c r="CW4" s="105"/>
-      <c r="CX4" s="105"/>
-      <c r="CY4" s="105"/>
-      <c r="CZ4" s="105"/>
-      <c r="DA4" s="105"/>
-      <c r="DB4" s="106"/>
-      <c r="DC4" s="104">
+      <c r="CW4" s="108"/>
+      <c r="CX4" s="108"/>
+      <c r="CY4" s="108"/>
+      <c r="CZ4" s="108"/>
+      <c r="DA4" s="108"/>
+      <c r="DB4" s="109"/>
+      <c r="DC4" s="107">
         <f t="shared" ref="DC4" si="0">DC5</f>
         <v>44949</v>
       </c>
-      <c r="DD4" s="105"/>
-      <c r="DE4" s="105"/>
-      <c r="DF4" s="105"/>
-      <c r="DG4" s="105"/>
-      <c r="DH4" s="105"/>
-      <c r="DI4" s="106"/>
-      <c r="DJ4" s="104">
+      <c r="DD4" s="108"/>
+      <c r="DE4" s="108"/>
+      <c r="DF4" s="108"/>
+      <c r="DG4" s="108"/>
+      <c r="DH4" s="108"/>
+      <c r="DI4" s="109"/>
+      <c r="DJ4" s="107">
         <f t="shared" ref="DJ4" si="1">DJ5</f>
         <v>44956</v>
       </c>
-      <c r="DK4" s="105"/>
-      <c r="DL4" s="105"/>
-      <c r="DM4" s="105"/>
-      <c r="DN4" s="105"/>
-      <c r="DO4" s="105"/>
-      <c r="DP4" s="106"/>
-      <c r="DQ4" s="104">
+      <c r="DK4" s="108"/>
+      <c r="DL4" s="108"/>
+      <c r="DM4" s="108"/>
+      <c r="DN4" s="108"/>
+      <c r="DO4" s="108"/>
+      <c r="DP4" s="109"/>
+      <c r="DQ4" s="107">
         <f t="shared" ref="DQ4" si="2">DQ5</f>
         <v>44963</v>
       </c>
-      <c r="DR4" s="105"/>
-      <c r="DS4" s="105"/>
-      <c r="DT4" s="105"/>
-      <c r="DU4" s="105"/>
-      <c r="DV4" s="105"/>
-      <c r="DW4" s="106"/>
-      <c r="DX4" s="104">
+      <c r="DR4" s="108"/>
+      <c r="DS4" s="108"/>
+      <c r="DT4" s="108"/>
+      <c r="DU4" s="108"/>
+      <c r="DV4" s="108"/>
+      <c r="DW4" s="109"/>
+      <c r="DX4" s="107">
         <f t="shared" ref="DX4" si="3">DX5</f>
         <v>44970</v>
       </c>
-      <c r="DY4" s="105"/>
-      <c r="DZ4" s="105"/>
-      <c r="EA4" s="105"/>
-      <c r="EB4" s="105"/>
-      <c r="EC4" s="105"/>
-      <c r="ED4" s="106"/>
-      <c r="EE4" s="104">
+      <c r="DY4" s="108"/>
+      <c r="DZ4" s="108"/>
+      <c r="EA4" s="108"/>
+      <c r="EB4" s="108"/>
+      <c r="EC4" s="108"/>
+      <c r="ED4" s="109"/>
+      <c r="EE4" s="107">
         <f t="shared" ref="EE4" si="4">EE5</f>
         <v>44977</v>
       </c>
-      <c r="EF4" s="105"/>
-      <c r="EG4" s="105"/>
-      <c r="EH4" s="105"/>
-      <c r="EI4" s="105"/>
-      <c r="EJ4" s="105"/>
-      <c r="EK4" s="106"/>
-      <c r="EL4" s="104">
+      <c r="EF4" s="108"/>
+      <c r="EG4" s="108"/>
+      <c r="EH4" s="108"/>
+      <c r="EI4" s="108"/>
+      <c r="EJ4" s="108"/>
+      <c r="EK4" s="109"/>
+      <c r="EL4" s="107">
         <f t="shared" ref="EL4" si="5">EL5</f>
         <v>44984</v>
       </c>
-      <c r="EM4" s="105"/>
-      <c r="EN4" s="105"/>
-      <c r="EO4" s="105"/>
-      <c r="EP4" s="105"/>
-      <c r="EQ4" s="105"/>
-      <c r="ER4" s="106"/>
-      <c r="ES4" s="104">
+      <c r="EM4" s="108"/>
+      <c r="EN4" s="108"/>
+      <c r="EO4" s="108"/>
+      <c r="EP4" s="108"/>
+      <c r="EQ4" s="108"/>
+      <c r="ER4" s="109"/>
+      <c r="ES4" s="107">
         <f t="shared" ref="ES4" si="6">ES5</f>
         <v>44991</v>
       </c>
-      <c r="ET4" s="105"/>
-      <c r="EU4" s="105"/>
-      <c r="EV4" s="105"/>
-      <c r="EW4" s="105"/>
-      <c r="EX4" s="105"/>
-      <c r="EY4" s="106"/>
-      <c r="EZ4" s="104">
+      <c r="ET4" s="108"/>
+      <c r="EU4" s="108"/>
+      <c r="EV4" s="108"/>
+      <c r="EW4" s="108"/>
+      <c r="EX4" s="108"/>
+      <c r="EY4" s="109"/>
+      <c r="EZ4" s="107">
         <f t="shared" ref="EZ4" si="7">EZ5</f>
         <v>44998</v>
       </c>
-      <c r="FA4" s="105"/>
-      <c r="FB4" s="105"/>
-      <c r="FC4" s="105"/>
-      <c r="FD4" s="105"/>
-      <c r="FE4" s="105"/>
-      <c r="FF4" s="106"/>
-      <c r="FG4" s="104">
+      <c r="FA4" s="108"/>
+      <c r="FB4" s="108"/>
+      <c r="FC4" s="108"/>
+      <c r="FD4" s="108"/>
+      <c r="FE4" s="108"/>
+      <c r="FF4" s="109"/>
+      <c r="FG4" s="107">
         <f t="shared" ref="FG4" si="8">FG5</f>
         <v>45005</v>
       </c>
-      <c r="FH4" s="105"/>
-      <c r="FI4" s="105"/>
-      <c r="FJ4" s="105"/>
-      <c r="FK4" s="105"/>
-      <c r="FL4" s="105"/>
-      <c r="FM4" s="106"/>
-      <c r="FN4" s="104">
+      <c r="FH4" s="108"/>
+      <c r="FI4" s="108"/>
+      <c r="FJ4" s="108"/>
+      <c r="FK4" s="108"/>
+      <c r="FL4" s="108"/>
+      <c r="FM4" s="109"/>
+      <c r="FN4" s="107">
         <f t="shared" ref="FN4" si="9">FN5</f>
         <v>45012</v>
       </c>
-      <c r="FO4" s="105"/>
-      <c r="FP4" s="105"/>
-      <c r="FQ4" s="105"/>
-      <c r="FR4" s="105"/>
-      <c r="FS4" s="105"/>
-      <c r="FT4" s="106"/>
-      <c r="FU4" s="104">
+      <c r="FO4" s="108"/>
+      <c r="FP4" s="108"/>
+      <c r="FQ4" s="108"/>
+      <c r="FR4" s="108"/>
+      <c r="FS4" s="108"/>
+      <c r="FT4" s="109"/>
+      <c r="FU4" s="107">
         <f t="shared" ref="FU4" si="10">FU5</f>
         <v>45019</v>
       </c>
-      <c r="FV4" s="105"/>
-      <c r="FW4" s="105"/>
-      <c r="FX4" s="105"/>
-      <c r="FY4" s="105"/>
-      <c r="FZ4" s="105"/>
-      <c r="GA4" s="106"/>
-      <c r="GB4" s="104">
+      <c r="FV4" s="108"/>
+      <c r="FW4" s="108"/>
+      <c r="FX4" s="108"/>
+      <c r="FY4" s="108"/>
+      <c r="FZ4" s="108"/>
+      <c r="GA4" s="109"/>
+      <c r="GB4" s="107">
         <f t="shared" ref="GB4" si="11">GB5</f>
         <v>45026</v>
       </c>
-      <c r="GC4" s="105"/>
-      <c r="GD4" s="105"/>
-      <c r="GE4" s="105"/>
-      <c r="GF4" s="105"/>
-      <c r="GG4" s="105"/>
-      <c r="GH4" s="106"/>
-      <c r="GI4" s="104">
+      <c r="GC4" s="108"/>
+      <c r="GD4" s="108"/>
+      <c r="GE4" s="108"/>
+      <c r="GF4" s="108"/>
+      <c r="GG4" s="108"/>
+      <c r="GH4" s="109"/>
+      <c r="GI4" s="107">
         <f t="shared" ref="GI4" si="12">GI5</f>
         <v>45033</v>
       </c>
-      <c r="GJ4" s="105"/>
-      <c r="GK4" s="105"/>
-      <c r="GL4" s="105"/>
-      <c r="GM4" s="105"/>
-      <c r="GN4" s="105"/>
-      <c r="GO4" s="106"/>
-      <c r="GP4" s="104">
+      <c r="GJ4" s="108"/>
+      <c r="GK4" s="108"/>
+      <c r="GL4" s="108"/>
+      <c r="GM4" s="108"/>
+      <c r="GN4" s="108"/>
+      <c r="GO4" s="109"/>
+      <c r="GP4" s="107">
         <f t="shared" ref="GP4" si="13">GP5</f>
         <v>45040</v>
       </c>
-      <c r="GQ4" s="105"/>
-      <c r="GR4" s="105"/>
-      <c r="GS4" s="105"/>
-      <c r="GT4" s="105"/>
-      <c r="GU4" s="105"/>
-      <c r="GV4" s="106"/>
-      <c r="GW4" s="104">
+      <c r="GQ4" s="108"/>
+      <c r="GR4" s="108"/>
+      <c r="GS4" s="108"/>
+      <c r="GT4" s="108"/>
+      <c r="GU4" s="108"/>
+      <c r="GV4" s="109"/>
+      <c r="GW4" s="107">
         <f t="shared" ref="GW4" si="14">GW5</f>
         <v>45047</v>
       </c>
-      <c r="GX4" s="105"/>
-      <c r="GY4" s="105"/>
-      <c r="GZ4" s="105"/>
-      <c r="HA4" s="105"/>
-      <c r="HB4" s="105"/>
-      <c r="HC4" s="106"/>
+      <c r="GX4" s="108"/>
+      <c r="GY4" s="108"/>
+      <c r="GZ4" s="108"/>
+      <c r="HA4" s="108"/>
+      <c r="HB4" s="108"/>
+      <c r="HC4" s="109"/>
     </row>
     <row r="5" spans="1:212" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="35" t="s">
@@ -4310,7 +4304,7 @@
       <c r="F8" s="57"/>
       <c r="G8" s="13"/>
       <c r="H8" s="13" t="str">
-        <f t="shared" ref="H8:H47" si="143">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H49" si="143">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="30"/>
@@ -10626,20 +10620,19 @@
       <c r="B36" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="C36" s="81" t="s">
-        <v>42</v>
+      <c r="C36" s="80" t="s">
+        <v>74</v>
       </c>
       <c r="D36" s="25">
-        <f>AVERAGE(D27:D35)</f>
         <v>0</v>
       </c>
       <c r="E36" s="67">
-        <f>E28</f>
-        <v>44912</v>
+        <f>F35+1</f>
+        <v>44998</v>
       </c>
       <c r="F36" s="67">
-        <f>F35</f>
-        <v>44997</v>
+        <f>E36+7</f>
+        <v>45005</v>
       </c>
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
@@ -10849,13 +10842,24 @@
     </row>
     <row r="37" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="34"/>
-      <c r="B37" s="83" t="s">
-        <v>57</v>
-      </c>
-      <c r="C37" s="82"/>
-      <c r="D37" s="84"/>
-      <c r="E37" s="85"/>
-      <c r="F37" s="85"/>
+      <c r="B37" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" s="81" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" s="25">
+        <f>AVERAGE(D27:D36)</f>
+        <v>0</v>
+      </c>
+      <c r="E37" s="67">
+        <f>E28</f>
+        <v>44912</v>
+      </c>
+      <c r="F37" s="67">
+        <f>F36</f>
+        <v>45005</v>
+      </c>
       <c r="G37" s="13"/>
       <c r="H37" s="13"/>
       <c r="I37" s="30"/>
@@ -11064,23 +11068,13 @@
     </row>
     <row r="38" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="34"/>
-      <c r="B38" s="87" t="s">
-        <v>15</v>
-      </c>
-      <c r="C38" s="88" t="s">
-        <v>58</v>
-      </c>
-      <c r="D38" s="89">
-        <v>0</v>
-      </c>
-      <c r="E38" s="90">
-        <f>F36+1</f>
-        <v>44998</v>
-      </c>
-      <c r="F38" s="90">
-        <f>E38+7</f>
-        <v>45005</v>
-      </c>
+      <c r="B38" s="83" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" s="82"/>
+      <c r="D38" s="84"/>
+      <c r="E38" s="85"/>
+      <c r="F38" s="85"/>
       <c r="G38" s="13"/>
       <c r="H38" s="13"/>
       <c r="I38" s="30"/>
@@ -11290,21 +11284,21 @@
     <row r="39" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="34"/>
       <c r="B39" s="87" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C39" s="88" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D39" s="89">
         <v>0</v>
       </c>
       <c r="E39" s="90">
-        <f>F38+1</f>
+        <f>F37+1</f>
         <v>45006</v>
       </c>
       <c r="F39" s="90">
-        <f>E39+5</f>
-        <v>45011</v>
+        <f>E39+7</f>
+        <v>45013</v>
       </c>
       <c r="G39" s="13"/>
       <c r="H39" s="13"/>
@@ -11515,21 +11509,21 @@
     <row r="40" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="34"/>
       <c r="B40" s="87" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C40" s="88" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D40" s="89">
         <v>0</v>
       </c>
       <c r="E40" s="90">
         <f>F39+1</f>
-        <v>45012</v>
+        <v>45014</v>
       </c>
       <c r="F40" s="90">
-        <f>E40+3</f>
-        <v>45015</v>
+        <f>E40+5</f>
+        <v>45019</v>
       </c>
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
@@ -11740,22 +11734,21 @@
     <row r="41" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="34"/>
       <c r="B41" s="87" t="s">
-        <v>18</v>
-      </c>
-      <c r="C41" s="86" t="s">
-        <v>57</v>
+        <v>17</v>
+      </c>
+      <c r="C41" s="88" t="s">
+        <v>60</v>
       </c>
       <c r="D41" s="89">
-        <f>AVERAGE(D38:D40)</f>
         <v>0</v>
       </c>
       <c r="E41" s="90">
-        <f>E38</f>
-        <v>44998</v>
+        <f>F40+1</f>
+        <v>45020</v>
       </c>
       <c r="F41" s="90">
-        <f>F40</f>
-        <v>45015</v>
+        <f>E41+3</f>
+        <v>45023</v>
       </c>
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
@@ -11965,13 +11958,24 @@
     </row>
     <row r="42" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="34"/>
-      <c r="B42" s="94" t="s">
-        <v>61</v>
-      </c>
-      <c r="C42" s="91"/>
-      <c r="D42" s="92"/>
-      <c r="E42" s="93"/>
-      <c r="F42" s="93"/>
+      <c r="B42" s="87" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="D42" s="89">
+        <f>AVERAGE(D39:D41)</f>
+        <v>0</v>
+      </c>
+      <c r="E42" s="90">
+        <f>E39</f>
+        <v>45006</v>
+      </c>
+      <c r="F42" s="90">
+        <f>F41</f>
+        <v>45023</v>
+      </c>
       <c r="G42" s="13"/>
       <c r="H42" s="13"/>
       <c r="I42" s="30"/>
@@ -12180,23 +12184,13 @@
     </row>
     <row r="43" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="34"/>
-      <c r="B43" s="98" t="s">
-        <v>15</v>
-      </c>
-      <c r="C43" s="99" t="s">
-        <v>62</v>
-      </c>
-      <c r="D43" s="96">
-        <v>0</v>
-      </c>
-      <c r="E43" s="97">
-        <f>F41+1</f>
-        <v>45016</v>
-      </c>
-      <c r="F43" s="97">
-        <f>E43+3</f>
-        <v>45019</v>
-      </c>
+      <c r="B43" s="94" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" s="91"/>
+      <c r="D43" s="92"/>
+      <c r="E43" s="93"/>
+      <c r="F43" s="93"/>
       <c r="G43" s="13"/>
       <c r="H43" s="13"/>
       <c r="I43" s="30"/>
@@ -12406,21 +12400,21 @@
     <row r="44" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="34"/>
       <c r="B44" s="98" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C44" s="99" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D44" s="96">
         <v>0</v>
       </c>
       <c r="E44" s="97">
-        <f>F43+1</f>
-        <v>45020</v>
+        <f>F42+1</f>
+        <v>45024</v>
       </c>
       <c r="F44" s="97">
         <f>E44+3</f>
-        <v>45023</v>
+        <v>45027</v>
       </c>
       <c r="G44" s="13"/>
       <c r="H44" s="13"/>
@@ -12631,21 +12625,21 @@
     <row r="45" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="34"/>
       <c r="B45" s="98" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C45" s="99" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D45" s="96">
         <v>0</v>
       </c>
       <c r="E45" s="97">
         <f>F44+1</f>
-        <v>45024</v>
+        <v>45028</v>
       </c>
       <c r="F45" s="97">
-        <f>E45+5</f>
-        <v>45029</v>
+        <f>E45+3</f>
+        <v>45031</v>
       </c>
       <c r="G45" s="13"/>
       <c r="H45" s="13"/>
@@ -12856,22 +12850,21 @@
     <row r="46" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="34"/>
       <c r="B46" s="98" t="s">
-        <v>18</v>
-      </c>
-      <c r="C46" s="95" t="s">
-        <v>65</v>
+        <v>17</v>
+      </c>
+      <c r="C46" s="99" t="s">
+        <v>63</v>
       </c>
       <c r="D46" s="96">
-        <f>AVERAGE(D43:D45)</f>
         <v>0</v>
       </c>
       <c r="E46" s="97">
-        <f>E43</f>
-        <v>45016</v>
+        <f>F45+1</f>
+        <v>45032</v>
       </c>
       <c r="F46" s="97">
-        <f>F45</f>
-        <v>45029</v>
+        <f>E46+5</f>
+        <v>45037</v>
       </c>
       <c r="G46" s="13"/>
       <c r="H46" s="13"/>
@@ -13080,237 +13073,701 @@
       <c r="HC46" s="30"/>
     </row>
     <row r="47" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="35" t="s">
+      <c r="A47" s="34"/>
+      <c r="B47" s="98" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" s="95" t="s">
+        <v>65</v>
+      </c>
+      <c r="D47" s="96">
+        <f>AVERAGE(D44:D46)</f>
+        <v>0</v>
+      </c>
+      <c r="E47" s="97">
+        <f>E44</f>
+        <v>45024</v>
+      </c>
+      <c r="F47" s="97">
+        <f>F46</f>
+        <v>45037</v>
+      </c>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="30"/>
+      <c r="J47" s="30"/>
+      <c r="K47" s="30"/>
+      <c r="L47" s="30"/>
+      <c r="M47" s="30"/>
+      <c r="N47" s="30"/>
+      <c r="O47" s="30"/>
+      <c r="P47" s="30"/>
+      <c r="Q47" s="30"/>
+      <c r="R47" s="30"/>
+      <c r="S47" s="30"/>
+      <c r="T47" s="30"/>
+      <c r="U47" s="30"/>
+      <c r="V47" s="30"/>
+      <c r="W47" s="30"/>
+      <c r="X47" s="30"/>
+      <c r="Y47" s="30"/>
+      <c r="Z47" s="30"/>
+      <c r="AA47" s="30"/>
+      <c r="AB47" s="30"/>
+      <c r="AC47" s="30"/>
+      <c r="AD47" s="30"/>
+      <c r="AE47" s="30"/>
+      <c r="AF47" s="30"/>
+      <c r="AG47" s="30"/>
+      <c r="AH47" s="30"/>
+      <c r="AI47" s="30"/>
+      <c r="AJ47" s="30"/>
+      <c r="AK47" s="30"/>
+      <c r="AL47" s="30"/>
+      <c r="AM47" s="30"/>
+      <c r="AN47" s="30"/>
+      <c r="AO47" s="30"/>
+      <c r="AP47" s="30"/>
+      <c r="AQ47" s="30"/>
+      <c r="AR47" s="30"/>
+      <c r="AS47" s="30"/>
+      <c r="AT47" s="30"/>
+      <c r="AU47" s="30"/>
+      <c r="AV47" s="30"/>
+      <c r="AW47" s="30"/>
+      <c r="AX47" s="30"/>
+      <c r="AY47" s="30"/>
+      <c r="AZ47" s="30"/>
+      <c r="BA47" s="30"/>
+      <c r="BB47" s="30"/>
+      <c r="BC47" s="30"/>
+      <c r="BD47" s="30"/>
+      <c r="BE47" s="30"/>
+      <c r="BF47" s="30"/>
+      <c r="BG47" s="30"/>
+      <c r="BH47" s="30"/>
+      <c r="BI47" s="30"/>
+      <c r="BJ47" s="30"/>
+      <c r="BK47" s="30"/>
+      <c r="BL47" s="30"/>
+      <c r="BM47" s="30"/>
+      <c r="BN47" s="101"/>
+      <c r="BO47" s="30"/>
+      <c r="BP47" s="30"/>
+      <c r="BQ47" s="30"/>
+      <c r="BR47" s="30"/>
+      <c r="BS47" s="30"/>
+      <c r="BT47" s="30"/>
+      <c r="BU47" s="30"/>
+      <c r="BV47" s="30"/>
+      <c r="BW47" s="30"/>
+      <c r="BX47" s="30"/>
+      <c r="BY47" s="30"/>
+      <c r="BZ47" s="30"/>
+      <c r="CA47" s="30"/>
+      <c r="CB47" s="30"/>
+      <c r="CC47" s="30"/>
+      <c r="CD47" s="30"/>
+      <c r="CE47" s="30"/>
+      <c r="CF47" s="30"/>
+      <c r="CG47" s="30"/>
+      <c r="CH47" s="30"/>
+      <c r="CI47" s="30"/>
+      <c r="CJ47" s="30"/>
+      <c r="CK47" s="30"/>
+      <c r="CL47" s="30"/>
+      <c r="CM47" s="30"/>
+      <c r="CN47" s="30"/>
+      <c r="CO47" s="30"/>
+      <c r="CP47" s="30"/>
+      <c r="CQ47" s="30"/>
+      <c r="CR47" s="30"/>
+      <c r="CS47" s="30"/>
+      <c r="CT47" s="30"/>
+      <c r="CU47" s="30"/>
+      <c r="CV47" s="30"/>
+      <c r="CW47" s="30"/>
+      <c r="CX47" s="30"/>
+      <c r="CY47" s="30"/>
+      <c r="CZ47" s="30"/>
+      <c r="DA47" s="30"/>
+      <c r="DB47" s="30"/>
+      <c r="DC47" s="30"/>
+      <c r="DD47" s="30"/>
+      <c r="DE47" s="30"/>
+      <c r="DF47" s="30"/>
+      <c r="DG47" s="30"/>
+      <c r="DH47" s="30"/>
+      <c r="DI47" s="30"/>
+      <c r="DJ47" s="30"/>
+      <c r="DK47" s="30"/>
+      <c r="DL47" s="30"/>
+      <c r="DM47" s="30"/>
+      <c r="DN47" s="30"/>
+      <c r="DO47" s="30"/>
+      <c r="DP47" s="30"/>
+      <c r="DQ47" s="30"/>
+      <c r="DR47" s="30"/>
+      <c r="DS47" s="30"/>
+      <c r="DT47" s="30"/>
+      <c r="DU47" s="30"/>
+      <c r="DV47" s="30"/>
+      <c r="DW47" s="30"/>
+      <c r="DX47" s="30"/>
+      <c r="DY47" s="30"/>
+      <c r="DZ47" s="30"/>
+      <c r="EA47" s="30"/>
+      <c r="EB47" s="30"/>
+      <c r="EC47" s="30"/>
+      <c r="ED47" s="30"/>
+      <c r="EE47" s="30"/>
+      <c r="EF47" s="30"/>
+      <c r="EG47" s="30"/>
+      <c r="EH47" s="30"/>
+      <c r="EI47" s="30"/>
+      <c r="EJ47" s="30"/>
+      <c r="EK47" s="30"/>
+      <c r="EL47" s="30"/>
+      <c r="EM47" s="30"/>
+      <c r="EN47" s="30"/>
+      <c r="EO47" s="30"/>
+      <c r="EP47" s="30"/>
+      <c r="EQ47" s="30"/>
+      <c r="ER47" s="30"/>
+      <c r="ES47" s="30"/>
+      <c r="ET47" s="30"/>
+      <c r="EU47" s="30"/>
+      <c r="EV47" s="30"/>
+      <c r="EW47" s="30"/>
+      <c r="EX47" s="30"/>
+      <c r="EY47" s="30"/>
+      <c r="EZ47" s="30"/>
+      <c r="FA47" s="30"/>
+      <c r="FB47" s="30"/>
+      <c r="FC47" s="30"/>
+      <c r="FD47" s="30"/>
+      <c r="FE47" s="30"/>
+      <c r="FF47" s="30"/>
+      <c r="FG47" s="30"/>
+      <c r="FH47" s="30"/>
+      <c r="FI47" s="30"/>
+      <c r="FJ47" s="30"/>
+      <c r="FK47" s="30"/>
+      <c r="FL47" s="30"/>
+      <c r="FM47" s="30"/>
+      <c r="FN47" s="30"/>
+      <c r="FO47" s="30"/>
+      <c r="FP47" s="30"/>
+      <c r="FQ47" s="30"/>
+      <c r="FR47" s="30"/>
+      <c r="FS47" s="30"/>
+      <c r="FT47" s="30"/>
+      <c r="FU47" s="30"/>
+      <c r="FV47" s="30"/>
+      <c r="FW47" s="30"/>
+      <c r="FX47" s="30"/>
+      <c r="FY47" s="30"/>
+      <c r="FZ47" s="30"/>
+      <c r="GA47" s="30"/>
+      <c r="GB47" s="30"/>
+      <c r="GC47" s="30"/>
+      <c r="GD47" s="30"/>
+      <c r="GE47" s="30"/>
+      <c r="GF47" s="30"/>
+      <c r="GG47" s="30"/>
+      <c r="GH47" s="30"/>
+      <c r="GI47" s="30"/>
+      <c r="GJ47" s="30"/>
+      <c r="GK47" s="30"/>
+      <c r="GL47" s="30"/>
+      <c r="GM47" s="30"/>
+      <c r="GN47" s="30"/>
+      <c r="GO47" s="30"/>
+      <c r="GP47" s="30"/>
+      <c r="GQ47" s="30"/>
+      <c r="GR47" s="30"/>
+      <c r="GS47" s="30"/>
+      <c r="GT47" s="30"/>
+      <c r="GU47" s="30"/>
+      <c r="GV47" s="30"/>
+      <c r="GW47" s="30"/>
+      <c r="GX47" s="75"/>
+      <c r="GY47" s="30"/>
+      <c r="GZ47" s="30"/>
+      <c r="HA47" s="30"/>
+      <c r="HB47" s="30"/>
+      <c r="HC47" s="30"/>
+    </row>
+    <row r="48" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="34"/>
+      <c r="B48" s="115" t="s">
+        <v>73</v>
+      </c>
+      <c r="C48" s="112"/>
+      <c r="D48" s="113"/>
+      <c r="E48" s="114">
+        <f>E27</f>
+        <v>44909</v>
+      </c>
+      <c r="F48" s="114">
+        <v>45048</v>
+      </c>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="30"/>
+      <c r="J48" s="30"/>
+      <c r="K48" s="30"/>
+      <c r="L48" s="30"/>
+      <c r="M48" s="30"/>
+      <c r="N48" s="30"/>
+      <c r="O48" s="30"/>
+      <c r="P48" s="30"/>
+      <c r="Q48" s="30"/>
+      <c r="R48" s="30"/>
+      <c r="S48" s="30"/>
+      <c r="T48" s="30"/>
+      <c r="U48" s="30"/>
+      <c r="V48" s="30"/>
+      <c r="W48" s="30"/>
+      <c r="X48" s="30"/>
+      <c r="Y48" s="30"/>
+      <c r="Z48" s="30"/>
+      <c r="AA48" s="30"/>
+      <c r="AB48" s="30"/>
+      <c r="AC48" s="30"/>
+      <c r="AD48" s="30"/>
+      <c r="AE48" s="30"/>
+      <c r="AF48" s="30"/>
+      <c r="AG48" s="30"/>
+      <c r="AH48" s="30"/>
+      <c r="AI48" s="30"/>
+      <c r="AJ48" s="30"/>
+      <c r="AK48" s="30"/>
+      <c r="AL48" s="30"/>
+      <c r="AM48" s="30"/>
+      <c r="AN48" s="30"/>
+      <c r="AO48" s="30"/>
+      <c r="AP48" s="30"/>
+      <c r="AQ48" s="30"/>
+      <c r="AR48" s="30"/>
+      <c r="AS48" s="30"/>
+      <c r="AT48" s="30"/>
+      <c r="AU48" s="30"/>
+      <c r="AV48" s="30"/>
+      <c r="AW48" s="30"/>
+      <c r="AX48" s="30"/>
+      <c r="AY48" s="30"/>
+      <c r="AZ48" s="30"/>
+      <c r="BA48" s="30"/>
+      <c r="BB48" s="30"/>
+      <c r="BC48" s="30"/>
+      <c r="BD48" s="30"/>
+      <c r="BE48" s="30"/>
+      <c r="BF48" s="30"/>
+      <c r="BG48" s="30"/>
+      <c r="BH48" s="30"/>
+      <c r="BI48" s="30"/>
+      <c r="BJ48" s="30"/>
+      <c r="BK48" s="30"/>
+      <c r="BL48" s="30"/>
+      <c r="BM48" s="30"/>
+      <c r="BN48" s="101"/>
+      <c r="BO48" s="30"/>
+      <c r="BP48" s="30"/>
+      <c r="BQ48" s="30"/>
+      <c r="BR48" s="30"/>
+      <c r="BS48" s="30"/>
+      <c r="BT48" s="30"/>
+      <c r="BU48" s="30"/>
+      <c r="BV48" s="30"/>
+      <c r="BW48" s="30"/>
+      <c r="BX48" s="30"/>
+      <c r="BY48" s="30"/>
+      <c r="BZ48" s="30"/>
+      <c r="CA48" s="30"/>
+      <c r="CB48" s="30"/>
+      <c r="CC48" s="30"/>
+      <c r="CD48" s="30"/>
+      <c r="CE48" s="30"/>
+      <c r="CF48" s="30"/>
+      <c r="CG48" s="30"/>
+      <c r="CH48" s="30"/>
+      <c r="CI48" s="30"/>
+      <c r="CJ48" s="30"/>
+      <c r="CK48" s="30"/>
+      <c r="CL48" s="30"/>
+      <c r="CM48" s="30"/>
+      <c r="CN48" s="30"/>
+      <c r="CO48" s="30"/>
+      <c r="CP48" s="30"/>
+      <c r="CQ48" s="30"/>
+      <c r="CR48" s="30"/>
+      <c r="CS48" s="30"/>
+      <c r="CT48" s="30"/>
+      <c r="CU48" s="30"/>
+      <c r="CV48" s="30"/>
+      <c r="CW48" s="30"/>
+      <c r="CX48" s="30"/>
+      <c r="CY48" s="30"/>
+      <c r="CZ48" s="30"/>
+      <c r="DA48" s="30"/>
+      <c r="DB48" s="30"/>
+      <c r="DC48" s="30"/>
+      <c r="DD48" s="30"/>
+      <c r="DE48" s="30"/>
+      <c r="DF48" s="30"/>
+      <c r="DG48" s="30"/>
+      <c r="DH48" s="30"/>
+      <c r="DI48" s="30"/>
+      <c r="DJ48" s="30"/>
+      <c r="DK48" s="30"/>
+      <c r="DL48" s="30"/>
+      <c r="DM48" s="30"/>
+      <c r="DN48" s="30"/>
+      <c r="DO48" s="30"/>
+      <c r="DP48" s="30"/>
+      <c r="DQ48" s="30"/>
+      <c r="DR48" s="30"/>
+      <c r="DS48" s="30"/>
+      <c r="DT48" s="30"/>
+      <c r="DU48" s="30"/>
+      <c r="DV48" s="30"/>
+      <c r="DW48" s="30"/>
+      <c r="DX48" s="30"/>
+      <c r="DY48" s="30"/>
+      <c r="DZ48" s="30"/>
+      <c r="EA48" s="30"/>
+      <c r="EB48" s="30"/>
+      <c r="EC48" s="30"/>
+      <c r="ED48" s="30"/>
+      <c r="EE48" s="30"/>
+      <c r="EF48" s="30"/>
+      <c r="EG48" s="30"/>
+      <c r="EH48" s="30"/>
+      <c r="EI48" s="30"/>
+      <c r="EJ48" s="30"/>
+      <c r="EK48" s="30"/>
+      <c r="EL48" s="30"/>
+      <c r="EM48" s="30"/>
+      <c r="EN48" s="30"/>
+      <c r="EO48" s="30"/>
+      <c r="EP48" s="30"/>
+      <c r="EQ48" s="30"/>
+      <c r="ER48" s="30"/>
+      <c r="ES48" s="30"/>
+      <c r="ET48" s="30"/>
+      <c r="EU48" s="30"/>
+      <c r="EV48" s="30"/>
+      <c r="EW48" s="30"/>
+      <c r="EX48" s="30"/>
+      <c r="EY48" s="30"/>
+      <c r="EZ48" s="30"/>
+      <c r="FA48" s="30"/>
+      <c r="FB48" s="30"/>
+      <c r="FC48" s="30"/>
+      <c r="FD48" s="30"/>
+      <c r="FE48" s="30"/>
+      <c r="FF48" s="30"/>
+      <c r="FG48" s="30"/>
+      <c r="FH48" s="30"/>
+      <c r="FI48" s="30"/>
+      <c r="FJ48" s="30"/>
+      <c r="FK48" s="30"/>
+      <c r="FL48" s="30"/>
+      <c r="FM48" s="30"/>
+      <c r="FN48" s="30"/>
+      <c r="FO48" s="30"/>
+      <c r="FP48" s="30"/>
+      <c r="FQ48" s="30"/>
+      <c r="FR48" s="30"/>
+      <c r="FS48" s="30"/>
+      <c r="FT48" s="30"/>
+      <c r="FU48" s="30"/>
+      <c r="FV48" s="30"/>
+      <c r="FW48" s="30"/>
+      <c r="FX48" s="30"/>
+      <c r="FY48" s="30"/>
+      <c r="FZ48" s="30"/>
+      <c r="GA48" s="30"/>
+      <c r="GB48" s="30"/>
+      <c r="GC48" s="30"/>
+      <c r="GD48" s="30"/>
+      <c r="GE48" s="30"/>
+      <c r="GF48" s="30"/>
+      <c r="GG48" s="30"/>
+      <c r="GH48" s="30"/>
+      <c r="GI48" s="30"/>
+      <c r="GJ48" s="30"/>
+      <c r="GK48" s="30"/>
+      <c r="GL48" s="30"/>
+      <c r="GM48" s="30"/>
+      <c r="GN48" s="30"/>
+      <c r="GO48" s="30"/>
+      <c r="GP48" s="30"/>
+      <c r="GQ48" s="30"/>
+      <c r="GR48" s="30"/>
+      <c r="GS48" s="30"/>
+      <c r="GT48" s="30"/>
+      <c r="GU48" s="30"/>
+      <c r="GV48" s="30"/>
+      <c r="GW48" s="30"/>
+      <c r="GX48" s="75"/>
+      <c r="GY48" s="30"/>
+      <c r="GZ48" s="30"/>
+      <c r="HA48" s="30"/>
+      <c r="HB48" s="30"/>
+      <c r="HC48" s="30"/>
+    </row>
+    <row r="49" spans="1:211" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B47" s="26" t="s">
+      <c r="B49" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C47" s="27"/>
-      <c r="D47" s="28"/>
-      <c r="E47" s="68"/>
-      <c r="F47" s="69"/>
-      <c r="G47" s="29"/>
-      <c r="H47" s="29" t="str">
+      <c r="C49" s="27"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="68"/>
+      <c r="F49" s="69"/>
+      <c r="G49" s="29"/>
+      <c r="H49" s="29" t="str">
         <f t="shared" si="143"/>
         <v/>
       </c>
-      <c r="I47" s="32"/>
-      <c r="J47" s="32"/>
-      <c r="K47" s="32"/>
-      <c r="L47" s="32"/>
-      <c r="M47" s="32"/>
-      <c r="N47" s="32"/>
-      <c r="O47" s="32"/>
-      <c r="P47" s="32"/>
-      <c r="Q47" s="32"/>
-      <c r="R47" s="32"/>
-      <c r="S47" s="32"/>
-      <c r="T47" s="32"/>
-      <c r="U47" s="32"/>
-      <c r="V47" s="32"/>
-      <c r="W47" s="32"/>
-      <c r="X47" s="32"/>
-      <c r="Y47" s="32"/>
-      <c r="Z47" s="32"/>
-      <c r="AA47" s="32"/>
-      <c r="AB47" s="32"/>
-      <c r="AC47" s="32"/>
-      <c r="AD47" s="32"/>
-      <c r="AE47" s="32"/>
-      <c r="AF47" s="32"/>
-      <c r="AG47" s="32"/>
-      <c r="AH47" s="32"/>
-      <c r="AI47" s="32"/>
-      <c r="AJ47" s="32"/>
-      <c r="AK47" s="32"/>
-      <c r="AL47" s="32"/>
-      <c r="AM47" s="32"/>
-      <c r="AN47" s="32"/>
-      <c r="AO47" s="32"/>
-      <c r="AP47" s="32"/>
-      <c r="AQ47" s="32"/>
-      <c r="AR47" s="32"/>
-      <c r="AS47" s="32"/>
-      <c r="AT47" s="32"/>
-      <c r="AU47" s="32"/>
-      <c r="AV47" s="32"/>
-      <c r="AW47" s="32"/>
-      <c r="AX47" s="32"/>
-      <c r="AY47" s="32"/>
-      <c r="AZ47" s="32"/>
-      <c r="BA47" s="32"/>
-      <c r="BB47" s="32"/>
-      <c r="BC47" s="32"/>
-      <c r="BD47" s="32"/>
-      <c r="BE47" s="32"/>
-      <c r="BF47" s="32"/>
-      <c r="BG47" s="32"/>
-      <c r="BH47" s="32"/>
-      <c r="BI47" s="32"/>
-      <c r="BJ47" s="32"/>
-      <c r="BK47" s="32"/>
-      <c r="BL47" s="32"/>
-      <c r="BM47" s="32"/>
-      <c r="BN47" s="101"/>
-      <c r="BO47" s="32"/>
-      <c r="BP47" s="32"/>
-      <c r="BQ47" s="32"/>
-      <c r="BR47" s="32"/>
-      <c r="BS47" s="32"/>
-      <c r="BT47" s="32"/>
-      <c r="BU47" s="32"/>
-      <c r="BV47" s="32"/>
-      <c r="BW47" s="32"/>
-      <c r="BX47" s="32"/>
-      <c r="BY47" s="32"/>
-      <c r="BZ47" s="32"/>
-      <c r="CA47" s="32"/>
-      <c r="CB47" s="32"/>
-      <c r="CC47" s="32"/>
-      <c r="CD47" s="32"/>
-      <c r="CE47" s="32"/>
-      <c r="CF47" s="32"/>
-      <c r="CG47" s="32"/>
-      <c r="CH47" s="32"/>
-      <c r="CI47" s="32"/>
-      <c r="CJ47" s="32"/>
-      <c r="CK47" s="32"/>
-      <c r="CL47" s="32"/>
-      <c r="CM47" s="32"/>
-      <c r="CN47" s="32"/>
-      <c r="CO47" s="32"/>
-      <c r="CP47" s="32"/>
-      <c r="CQ47" s="32"/>
-      <c r="CR47" s="32"/>
-      <c r="CS47" s="32"/>
-      <c r="CT47" s="32"/>
-      <c r="CU47" s="32"/>
-      <c r="CV47" s="32"/>
-      <c r="CW47" s="32"/>
-      <c r="CX47" s="32"/>
-      <c r="CY47" s="32"/>
-      <c r="CZ47" s="32"/>
-      <c r="DA47" s="32"/>
-      <c r="DB47" s="32"/>
-      <c r="DC47" s="32"/>
-      <c r="DD47" s="32"/>
-      <c r="DE47" s="32"/>
-      <c r="DF47" s="32"/>
-      <c r="DG47" s="32"/>
-      <c r="DH47" s="32"/>
-      <c r="DI47" s="32"/>
-      <c r="DJ47" s="32"/>
-      <c r="DK47" s="32"/>
-      <c r="DL47" s="32"/>
-      <c r="DM47" s="32"/>
-      <c r="DN47" s="32"/>
-      <c r="DO47" s="32"/>
-      <c r="DP47" s="32"/>
-      <c r="DQ47" s="32"/>
-      <c r="DR47" s="32"/>
-      <c r="DS47" s="32"/>
-      <c r="DT47" s="32"/>
-      <c r="DU47" s="32"/>
-      <c r="DV47" s="32"/>
-      <c r="DW47" s="32"/>
-      <c r="DX47" s="32"/>
-      <c r="DY47" s="32"/>
-      <c r="DZ47" s="32"/>
-      <c r="EA47" s="32"/>
-      <c r="EB47" s="32"/>
-      <c r="EC47" s="32"/>
-      <c r="ED47" s="32"/>
-      <c r="EE47" s="32"/>
-      <c r="EF47" s="32"/>
-      <c r="EG47" s="32"/>
-      <c r="EH47" s="32"/>
-      <c r="EI47" s="32"/>
-      <c r="EJ47" s="32"/>
-      <c r="EK47" s="32"/>
-      <c r="EL47" s="32"/>
-      <c r="EM47" s="32"/>
-      <c r="EN47" s="32"/>
-      <c r="EO47" s="32"/>
-      <c r="EP47" s="32"/>
-      <c r="EQ47" s="32"/>
-      <c r="ER47" s="32"/>
-      <c r="ES47" s="32"/>
-      <c r="ET47" s="32"/>
-      <c r="EU47" s="32"/>
-      <c r="EV47" s="32"/>
-      <c r="EW47" s="32"/>
-      <c r="EX47" s="32"/>
-      <c r="EY47" s="32"/>
-      <c r="EZ47" s="32"/>
-      <c r="FA47" s="32"/>
-      <c r="FB47" s="32"/>
-      <c r="FC47" s="32"/>
-      <c r="FD47" s="32"/>
-      <c r="FE47" s="32"/>
-      <c r="FF47" s="32"/>
-      <c r="FG47" s="32"/>
-      <c r="FH47" s="32"/>
-      <c r="FI47" s="32"/>
-      <c r="FJ47" s="32"/>
-      <c r="FK47" s="32"/>
-      <c r="FL47" s="32"/>
-      <c r="FM47" s="32"/>
-      <c r="FN47" s="32"/>
-      <c r="FO47" s="32"/>
-      <c r="FP47" s="32"/>
-      <c r="FQ47" s="32"/>
-      <c r="FR47" s="32"/>
-      <c r="FS47" s="32"/>
-      <c r="FT47" s="32"/>
-      <c r="FU47" s="32"/>
-      <c r="FV47" s="32"/>
-      <c r="FW47" s="32"/>
-      <c r="FX47" s="32"/>
-      <c r="FY47" s="32"/>
-      <c r="FZ47" s="32"/>
-      <c r="GA47" s="32"/>
-      <c r="GB47" s="32"/>
-      <c r="GC47" s="32"/>
-      <c r="GD47" s="32"/>
-      <c r="GE47" s="32"/>
-      <c r="GF47" s="32"/>
-      <c r="GG47" s="32"/>
-      <c r="GH47" s="32"/>
-      <c r="GI47" s="32"/>
-      <c r="GJ47" s="32"/>
-      <c r="GK47" s="32"/>
-      <c r="GL47" s="32"/>
-      <c r="GM47" s="32"/>
-      <c r="GN47" s="32"/>
-      <c r="GO47" s="32"/>
-      <c r="GP47" s="32"/>
-      <c r="GQ47" s="32"/>
-      <c r="GR47" s="32"/>
-      <c r="GS47" s="32"/>
-      <c r="GT47" s="32"/>
-      <c r="GU47" s="32"/>
-      <c r="GV47" s="32"/>
-      <c r="GW47" s="32"/>
-      <c r="GX47" s="75"/>
-      <c r="GY47" s="32"/>
-      <c r="GZ47" s="32"/>
-      <c r="HA47" s="32"/>
-      <c r="HB47" s="32"/>
-      <c r="HC47" s="32"/>
+      <c r="I49" s="32"/>
+      <c r="J49" s="32"/>
+      <c r="K49" s="32"/>
+      <c r="L49" s="32"/>
+      <c r="M49" s="32"/>
+      <c r="N49" s="32"/>
+      <c r="O49" s="32"/>
+      <c r="P49" s="32"/>
+      <c r="Q49" s="32"/>
+      <c r="R49" s="32"/>
+      <c r="S49" s="32"/>
+      <c r="T49" s="32"/>
+      <c r="U49" s="32"/>
+      <c r="V49" s="32"/>
+      <c r="W49" s="32"/>
+      <c r="X49" s="32"/>
+      <c r="Y49" s="32"/>
+      <c r="Z49" s="32"/>
+      <c r="AA49" s="32"/>
+      <c r="AB49" s="32"/>
+      <c r="AC49" s="32"/>
+      <c r="AD49" s="32"/>
+      <c r="AE49" s="32"/>
+      <c r="AF49" s="32"/>
+      <c r="AG49" s="32"/>
+      <c r="AH49" s="32"/>
+      <c r="AI49" s="32"/>
+      <c r="AJ49" s="32"/>
+      <c r="AK49" s="32"/>
+      <c r="AL49" s="32"/>
+      <c r="AM49" s="32"/>
+      <c r="AN49" s="32"/>
+      <c r="AO49" s="32"/>
+      <c r="AP49" s="32"/>
+      <c r="AQ49" s="32"/>
+      <c r="AR49" s="32"/>
+      <c r="AS49" s="32"/>
+      <c r="AT49" s="32"/>
+      <c r="AU49" s="32"/>
+      <c r="AV49" s="32"/>
+      <c r="AW49" s="32"/>
+      <c r="AX49" s="32"/>
+      <c r="AY49" s="32"/>
+      <c r="AZ49" s="32"/>
+      <c r="BA49" s="32"/>
+      <c r="BB49" s="32"/>
+      <c r="BC49" s="32"/>
+      <c r="BD49" s="32"/>
+      <c r="BE49" s="32"/>
+      <c r="BF49" s="32"/>
+      <c r="BG49" s="32"/>
+      <c r="BH49" s="32"/>
+      <c r="BI49" s="32"/>
+      <c r="BJ49" s="32"/>
+      <c r="BK49" s="32"/>
+      <c r="BL49" s="32"/>
+      <c r="BM49" s="32"/>
+      <c r="BN49" s="101"/>
+      <c r="BO49" s="32"/>
+      <c r="BP49" s="32"/>
+      <c r="BQ49" s="32"/>
+      <c r="BR49" s="32"/>
+      <c r="BS49" s="32"/>
+      <c r="BT49" s="32"/>
+      <c r="BU49" s="32"/>
+      <c r="BV49" s="32"/>
+      <c r="BW49" s="32"/>
+      <c r="BX49" s="32"/>
+      <c r="BY49" s="32"/>
+      <c r="BZ49" s="32"/>
+      <c r="CA49" s="32"/>
+      <c r="CB49" s="32"/>
+      <c r="CC49" s="32"/>
+      <c r="CD49" s="32"/>
+      <c r="CE49" s="32"/>
+      <c r="CF49" s="32"/>
+      <c r="CG49" s="32"/>
+      <c r="CH49" s="32"/>
+      <c r="CI49" s="32"/>
+      <c r="CJ49" s="32"/>
+      <c r="CK49" s="32"/>
+      <c r="CL49" s="32"/>
+      <c r="CM49" s="32"/>
+      <c r="CN49" s="32"/>
+      <c r="CO49" s="32"/>
+      <c r="CP49" s="32"/>
+      <c r="CQ49" s="32"/>
+      <c r="CR49" s="32"/>
+      <c r="CS49" s="32"/>
+      <c r="CT49" s="32"/>
+      <c r="CU49" s="32"/>
+      <c r="CV49" s="32"/>
+      <c r="CW49" s="32"/>
+      <c r="CX49" s="32"/>
+      <c r="CY49" s="32"/>
+      <c r="CZ49" s="32"/>
+      <c r="DA49" s="32"/>
+      <c r="DB49" s="32"/>
+      <c r="DC49" s="32"/>
+      <c r="DD49" s="32"/>
+      <c r="DE49" s="32"/>
+      <c r="DF49" s="32"/>
+      <c r="DG49" s="32"/>
+      <c r="DH49" s="32"/>
+      <c r="DI49" s="32"/>
+      <c r="DJ49" s="32"/>
+      <c r="DK49" s="32"/>
+      <c r="DL49" s="32"/>
+      <c r="DM49" s="32"/>
+      <c r="DN49" s="32"/>
+      <c r="DO49" s="32"/>
+      <c r="DP49" s="32"/>
+      <c r="DQ49" s="32"/>
+      <c r="DR49" s="32"/>
+      <c r="DS49" s="32"/>
+      <c r="DT49" s="32"/>
+      <c r="DU49" s="32"/>
+      <c r="DV49" s="32"/>
+      <c r="DW49" s="32"/>
+      <c r="DX49" s="32"/>
+      <c r="DY49" s="32"/>
+      <c r="DZ49" s="32"/>
+      <c r="EA49" s="32"/>
+      <c r="EB49" s="32"/>
+      <c r="EC49" s="32"/>
+      <c r="ED49" s="32"/>
+      <c r="EE49" s="32"/>
+      <c r="EF49" s="32"/>
+      <c r="EG49" s="32"/>
+      <c r="EH49" s="32"/>
+      <c r="EI49" s="32"/>
+      <c r="EJ49" s="32"/>
+      <c r="EK49" s="32"/>
+      <c r="EL49" s="32"/>
+      <c r="EM49" s="32"/>
+      <c r="EN49" s="32"/>
+      <c r="EO49" s="32"/>
+      <c r="EP49" s="32"/>
+      <c r="EQ49" s="32"/>
+      <c r="ER49" s="32"/>
+      <c r="ES49" s="32"/>
+      <c r="ET49" s="32"/>
+      <c r="EU49" s="32"/>
+      <c r="EV49" s="32"/>
+      <c r="EW49" s="32"/>
+      <c r="EX49" s="32"/>
+      <c r="EY49" s="32"/>
+      <c r="EZ49" s="32"/>
+      <c r="FA49" s="32"/>
+      <c r="FB49" s="32"/>
+      <c r="FC49" s="32"/>
+      <c r="FD49" s="32"/>
+      <c r="FE49" s="32"/>
+      <c r="FF49" s="32"/>
+      <c r="FG49" s="32"/>
+      <c r="FH49" s="32"/>
+      <c r="FI49" s="32"/>
+      <c r="FJ49" s="32"/>
+      <c r="FK49" s="32"/>
+      <c r="FL49" s="32"/>
+      <c r="FM49" s="32"/>
+      <c r="FN49" s="32"/>
+      <c r="FO49" s="32"/>
+      <c r="FP49" s="32"/>
+      <c r="FQ49" s="32"/>
+      <c r="FR49" s="32"/>
+      <c r="FS49" s="32"/>
+      <c r="FT49" s="32"/>
+      <c r="FU49" s="32"/>
+      <c r="FV49" s="32"/>
+      <c r="FW49" s="32"/>
+      <c r="FX49" s="32"/>
+      <c r="FY49" s="32"/>
+      <c r="FZ49" s="32"/>
+      <c r="GA49" s="32"/>
+      <c r="GB49" s="32"/>
+      <c r="GC49" s="32"/>
+      <c r="GD49" s="32"/>
+      <c r="GE49" s="32"/>
+      <c r="GF49" s="32"/>
+      <c r="GG49" s="32"/>
+      <c r="GH49" s="32"/>
+      <c r="GI49" s="32"/>
+      <c r="GJ49" s="32"/>
+      <c r="GK49" s="32"/>
+      <c r="GL49" s="32"/>
+      <c r="GM49" s="32"/>
+      <c r="GN49" s="32"/>
+      <c r="GO49" s="32"/>
+      <c r="GP49" s="32"/>
+      <c r="GQ49" s="32"/>
+      <c r="GR49" s="32"/>
+      <c r="GS49" s="32"/>
+      <c r="GT49" s="32"/>
+      <c r="GU49" s="32"/>
+      <c r="GV49" s="32"/>
+      <c r="GW49" s="32"/>
+      <c r="GX49" s="75"/>
+      <c r="GY49" s="32"/>
+      <c r="GZ49" s="32"/>
+      <c r="HA49" s="32"/>
+      <c r="HB49" s="32"/>
+      <c r="HC49" s="32"/>
     </row>
-    <row r="48" spans="1:211" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G48" s="6"/>
+    <row r="50" spans="1:211" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G50" s="6"/>
     </row>
-    <row r="49" spans="3:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C49" s="11"/>
-      <c r="F49" s="36"/>
+    <row r="51" spans="1:211" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C51" s="11"/>
+      <c r="F51" s="36"/>
     </row>
-    <row r="50" spans="3:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C50" s="12"/>
+    <row r="52" spans="1:211" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C52" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="GI4:GO4"/>
+    <mergeCell ref="GP4:GV4"/>
+    <mergeCell ref="GW4:HC4"/>
+    <mergeCell ref="EZ4:FF4"/>
+    <mergeCell ref="FG4:FM4"/>
+    <mergeCell ref="FN4:FT4"/>
+    <mergeCell ref="FU4:GA4"/>
+    <mergeCell ref="GB4:GH4"/>
+    <mergeCell ref="DQ4:DW4"/>
+    <mergeCell ref="DX4:ED4"/>
+    <mergeCell ref="EE4:EK4"/>
+    <mergeCell ref="EL4:ER4"/>
+    <mergeCell ref="ES4:EY4"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="CO4:CU4"/>
     <mergeCell ref="GX2:HD2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
@@ -13327,27 +13784,9 @@
     <mergeCell ref="DC4:DI4"/>
     <mergeCell ref="DJ4:DP4"/>
     <mergeCell ref="BN2:BS2"/>
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="CO4:CU4"/>
-    <mergeCell ref="DQ4:DW4"/>
-    <mergeCell ref="DX4:ED4"/>
-    <mergeCell ref="EE4:EK4"/>
-    <mergeCell ref="EL4:ER4"/>
-    <mergeCell ref="ES4:EY4"/>
-    <mergeCell ref="GI4:GO4"/>
-    <mergeCell ref="GP4:GV4"/>
-    <mergeCell ref="GW4:HC4"/>
-    <mergeCell ref="EZ4:FF4"/>
-    <mergeCell ref="FG4:FM4"/>
-    <mergeCell ref="FN4:FT4"/>
-    <mergeCell ref="FU4:GA4"/>
-    <mergeCell ref="GB4:GH4"/>
   </mergeCells>
   <phoneticPr fontId="31" type="noConversion"/>
-  <conditionalFormatting sqref="D7:D11 D47 D13:D14 D28:D34 D16:D26">
+  <conditionalFormatting sqref="D7:D11 D49 D13:D14 D28:D34 D16:D26">
     <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -13361,12 +13800,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:HC47">
+  <conditionalFormatting sqref="I5:HC49">
     <cfRule type="expression" dxfId="3" priority="34">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:HC47">
+  <conditionalFormatting sqref="I7:HC49">
     <cfRule type="expression" dxfId="2" priority="20">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -13374,7 +13813,7 @@
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35:D46">
+  <conditionalFormatting sqref="D35:D48">
     <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -13430,7 +13869,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BN5:BN47">
+  <conditionalFormatting sqref="BN5:BN49">
     <cfRule type="expression" dxfId="0" priority="39">
       <formula>TRUE</formula>
     </cfRule>
@@ -13462,7 +13901,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D11 D47 D13:D14 D28:D34 D16:D26</xm:sqref>
+          <xm:sqref>D7:D11 D49 D13:D14 D28:D34 D16:D26</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{43BDC079-A4D3-4950-81E9-81F0EA5236AE}">
@@ -13477,7 +13916,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D35:D46</xm:sqref>
+          <xm:sqref>D35:D48</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C5B9DC40-6AA5-4EDE-985B-6615ABEB3CA0}">
@@ -13531,23 +13970,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaServiceKeyPoints xmlns="ade9cf8d-689b-44c7-83d3-1b6d2ed01456" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD32B88E8F5C5840BE58EFBF8C533A84" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eefc930e7d3d41296f1e209179b210f0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ade9cf8d-689b-44c7-83d3-1b6d2ed01456" xmlns:ns4="f2c43e5f-0c15-4f9b-b257-1465459d1450" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9fa27b00dd7b8e982819c8d20ed7c1fa" ns3:_="" ns4:_="">
     <xsd:import namespace="ade9cf8d-689b-44c7-83d3-1b6d2ed01456"/>
@@ -13750,32 +14172,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="f2c43e5f-0c15-4f9b-b257-1465459d1450"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="ade9cf8d-689b-44c7-83d3-1b6d2ed01456"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaServiceKeyPoints xmlns="ade9cf8d-689b-44c7-83d3-1b6d2ed01456" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB27BE46-3210-44BF-89A8-85069933A938}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13792,4 +14206,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="f2c43e5f-0c15-4f9b-b257-1465459d1450"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="ade9cf8d-689b-44c7-83d3-1b6d2ed01456"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>